<commit_message>
GQA - Avaliação (Quase Pronta)
</commit_message>
<xml_diff>
--- a/Raiz/Projeto/Avaliação/GQA-Avaliação Processo.xlsx
+++ b/Raiz/Projeto/Avaliação/GQA-Avaliação Processo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -357,6 +357,15 @@
   </si>
   <si>
     <t>Certificados da Garantia da Qualidade</t>
+  </si>
+  <si>
+    <t>Certificados</t>
+  </si>
+  <si>
+    <t>GQA - Especificação da Garantia da Qualidade (Tabela de Reuniões)</t>
+  </si>
+  <si>
+    <t>GQA - Documento de Integrantes</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1483,7 @@
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1539,7 +1548,7 @@
       <c r="C6" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1596,7 +1605,7 @@
       <c r="C13" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1649,7 +1658,7 @@
       <c r="C20" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1708,7 +1717,7 @@
       <c r="C28" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1905,7 +1914,7 @@
       <c r="C54" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1954,16 +1963,24 @@
       <c r="D60" s="24"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="23"/>
+      <c r="A61" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
+      <c r="D61" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="23"/>
+      <c r="A62" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
+      <c r="D62" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="23"/>
@@ -2001,7 +2018,7 @@
       <c r="C67" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D67" s="24" t="s">
+      <c r="D67" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2056,10 +2073,14 @@
       <c r="D74" s="24"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="23"/>
+      <c r="A75" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
+      <c r="D75" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="23"/>
@@ -2103,15 +2124,19 @@
       <c r="C81" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D81" s="24" t="s">
+      <c r="D81" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="23"/>
+      <c r="A82" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
+      <c r="D82" s="49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="23"/>
@@ -2155,6 +2180,17 @@
     <hyperlink ref="C74" r:id="rId9"/>
     <hyperlink ref="C54" r:id="rId10"/>
     <hyperlink ref="D7" r:id="rId11"/>
+    <hyperlink ref="D54" r:id="rId12"/>
+    <hyperlink ref="D67" r:id="rId13"/>
+    <hyperlink ref="D81" r:id="rId14"/>
+    <hyperlink ref="D13" r:id="rId15"/>
+    <hyperlink ref="D6" r:id="rId16"/>
+    <hyperlink ref="D82" r:id="rId17"/>
+    <hyperlink ref="D75" r:id="rId18"/>
+    <hyperlink ref="D61" r:id="rId19"/>
+    <hyperlink ref="D62" r:id="rId20"/>
+    <hyperlink ref="D28" r:id="rId21"/>
+    <hyperlink ref="D20" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>